<commit_message>
Updated DC Unit and added new methods for loading details after reopen
</commit_message>
<xml_diff>
--- a/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
+++ b/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E3353B-0145-4046-8C98-76ADC994DF67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4708EB61-102D-4A06-85B7-44733EAD0296}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t>Device</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t xml:space="preserve">NGC-1397 or NGC-595/TC-226 </t>
+  </si>
+  <si>
+    <t>DC Unit Loading Details Name</t>
+  </si>
+  <si>
+    <t>Current (DC Units)</t>
+  </si>
+  <si>
+    <t>Current (worst case)</t>
   </si>
 </sst>
 </file>
@@ -579,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,6 +623,9 @@
         <v>364.1</v>
       </c>
       <c r="H1" s="5"/>
+      <c r="I1" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="L1"/>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -629,6 +641,9 @@
       <c r="D2" s="20"/>
       <c r="F2" s="4"/>
       <c r="G2" s="8"/>
+      <c r="I2" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="L2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -647,6 +662,9 @@
       </c>
       <c r="G3" s="1">
         <v>5</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="L3"/>
     </row>
@@ -870,7 +888,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,6 +922,9 @@
         <v>411</v>
       </c>
       <c r="H1" s="3"/>
+      <c r="I1" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="72" x14ac:dyDescent="0.3">
@@ -923,6 +944,9 @@
       <c r="G2" s="8">
         <v>364.1</v>
       </c>
+      <c r="I2" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="12"/>
     </row>
@@ -942,6 +966,9 @@
       </c>
       <c r="G3" s="1">
         <v>5</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>

</xml_diff>

<commit_message>
Updated test data for TC-226
</commit_message>
<xml_diff>
--- a/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
+++ b/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
@@ -30,8 +30,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alpesh Dhakad</author>
+  </authors>
+  <commentList>
+    <comment ref="I8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+5BI 5" [517.050.018] &amp; 801RIL</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
   <si>
     <t>Device</t>
   </si>
@@ -147,9 +181,6 @@
     <t>LPAV 3000 - 4</t>
   </si>
   <si>
-    <t>5BI 5" [517.050.018] &amp; 801RIL</t>
-  </si>
-  <si>
     <t>DC Units on UI after adding device and Base</t>
   </si>
   <si>
@@ -178,13 +209,16 @@
   </si>
   <si>
     <t>Current (worst case)</t>
+  </si>
+  <si>
+    <t>Assign Base/Default Base Row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +240,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -584,11 +631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,14 +663,14 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="F1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="8">
         <v>364.1</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L1"/>
     </row>
@@ -632,7 +679,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>16</v>
@@ -641,7 +688,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="8"/>
       <c r="I2" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L2"/>
     </row>
@@ -650,7 +697,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="17" t="s">
@@ -663,7 +710,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3"/>
     </row>
@@ -672,7 +719,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="17" t="s">
@@ -722,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>18</v>
@@ -765,8 +812,8 @@
       <c r="H8" s="14">
         <v>1</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>38</v>
+      <c r="I8" s="13">
+        <v>11</v>
       </c>
       <c r="J8" s="13">
         <v>6</v>
@@ -809,8 +856,8 @@
       <c r="H9" s="14">
         <v>1.3</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>38</v>
+      <c r="I9" s="13">
+        <v>11</v>
       </c>
       <c r="J9" s="13">
         <v>6</v>
@@ -879,6 +926,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -886,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -915,14 +963,14 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="F1" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="8">
         <v>411</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" s="6"/>
     </row>
@@ -931,20 +979,20 @@
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="20"/>
       <c r="F2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="8">
         <v>364.1</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="12"/>
@@ -954,7 +1002,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="17" t="s">
@@ -967,7 +1015,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
@@ -977,7 +1025,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="17" t="s">
@@ -1101,7 +1149,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Updated test data for TC_226
</commit_message>
<xml_diff>
--- a/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
+++ b/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
@@ -37,6 +37,30 @@
   </authors>
   <commentList>
     <comment ref="I8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alpesh Dhakad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+5BI 5" [517.050.018] &amp; 801RIL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -634,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,7 +881,7 @@
         <v>1.3</v>
       </c>
       <c r="I9" s="13">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J9" s="13">
         <v>6</v>
@@ -934,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated test data for power calculation text and other base change related test cases
</commit_message>
<xml_diff>
--- a/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
+++ b/Test Data/TC_226_Verify Trip Current Calculation for PFI.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>Device</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>Assign Base/Default Base Row</t>
+  </si>
+  <si>
+    <t>LI800 - 1</t>
   </si>
 </sst>
 </file>
@@ -959,7 +962,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,7 +1220,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>12</v>

</xml_diff>